<commit_message>
Email portal style update and changes to modal
</commit_message>
<xml_diff>
--- a/public/assets/Email Upload Template.xlsx
+++ b/public/assets/Email Upload Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Padraig\Desktop\Computing Project\ComputingProject\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Padraig\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68626BBD-38F4-4938-A2F8-9FFDF29F85ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A991F701-85C1-4455-9BA7-C6B63A206C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D66E3EE3-C821-4D7B-9F29-F5B61556DA10}"/>
   </bookViews>
@@ -446,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF57300-6ADD-4B5B-8CE7-ADAABF44FE8A}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,7 +476,7 @@
     </row>
     <row r="2" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="3" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="6" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="7" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="8" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="9" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="10" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="11" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="12" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="13" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="14" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>7</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="15" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>7</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="16" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>7</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="17" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>7</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="18" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>7</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="19" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>7</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="20" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>7</v>
@@ -742,7 +742,7 @@
     </row>
     <row r="21" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="22" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>7</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="23" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
@@ -781,31 +781,34 @@
       <c r="D23" t="b">
         <v>1</v>
       </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F2DEA0FB-FED0-4704-B956-818CAC34A5BA}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{4692E147-837B-45B6-8B68-99B71174EF7B}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{78B200D7-3340-451B-A0E2-D385C9C49B16}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{DD8653D5-E242-4972-A0D5-CCC697CCB79C}"/>
-    <hyperlink ref="A8" r:id="rId5" xr:uid="{99740DC4-24A0-431B-9859-030FDD4A7A92}"/>
-    <hyperlink ref="A10" r:id="rId6" xr:uid="{BD0FB538-A669-478B-BB35-B488BE5258F3}"/>
-    <hyperlink ref="A12" r:id="rId7" xr:uid="{1AEF12FE-94E8-4D3E-A38F-85B26D2B42EB}"/>
-    <hyperlink ref="A14" r:id="rId8" xr:uid="{373279DF-52F7-4325-963D-2CFF1FC0CD82}"/>
-    <hyperlink ref="A16" r:id="rId9" xr:uid="{57BE27B6-C548-4657-86A6-0EB61F72CB40}"/>
-    <hyperlink ref="A18" r:id="rId10" xr:uid="{D371CDA2-2D04-4DD4-B225-87E802362E06}"/>
-    <hyperlink ref="A20" r:id="rId11" xr:uid="{FB0D88F6-92E3-4433-AEC6-F3F5297114BE}"/>
-    <hyperlink ref="A22" r:id="rId12" xr:uid="{F2D92F8D-E5D3-45D8-9262-2BFC159DC543}"/>
-    <hyperlink ref="A5" r:id="rId13" xr:uid="{B981A00F-221D-462C-B348-4B283B9F4D47}"/>
-    <hyperlink ref="A7" r:id="rId14" xr:uid="{9B175458-30E8-4938-8ABC-F7073D88621D}"/>
-    <hyperlink ref="A9" r:id="rId15" xr:uid="{7324B8EE-E890-4FBA-B1CF-09B764F7B2CC}"/>
-    <hyperlink ref="A11" r:id="rId16" xr:uid="{8D893167-B4BD-434C-8958-C827F23AC77B}"/>
-    <hyperlink ref="A13" r:id="rId17" xr:uid="{9475FAF3-B43C-4BC9-A052-8E4B3EABC24B}"/>
-    <hyperlink ref="A15" r:id="rId18" xr:uid="{5170F69E-34FA-47D6-AEEF-ADFDDE57687B}"/>
-    <hyperlink ref="A17" r:id="rId19" xr:uid="{CB62A601-E999-4D97-8576-41D4FBF024A8}"/>
-    <hyperlink ref="A19" r:id="rId20" xr:uid="{DD7284B4-1210-4865-B889-85C234B26328}"/>
-    <hyperlink ref="A21" r:id="rId21" xr:uid="{99B56FB7-25B4-49CA-B674-F186636B10D6}"/>
-    <hyperlink ref="A23" r:id="rId22" xr:uid="{7DF435F3-900F-4F66-8FD1-6A898FF06BD5}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{F2DEA0FB-FED0-4704-B956-818CAC34A5BA}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{4692E147-837B-45B6-8B68-99B71174EF7B}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{78B200D7-3340-451B-A0E2-D385C9C49B16}"/>
+    <hyperlink ref="A7" r:id="rId4" xr:uid="{DD8653D5-E242-4972-A0D5-CCC697CCB79C}"/>
+    <hyperlink ref="A9" r:id="rId5" xr:uid="{99740DC4-24A0-431B-9859-030FDD4A7A92}"/>
+    <hyperlink ref="A11" r:id="rId6" xr:uid="{BD0FB538-A669-478B-BB35-B488BE5258F3}"/>
+    <hyperlink ref="A13" r:id="rId7" xr:uid="{1AEF12FE-94E8-4D3E-A38F-85B26D2B42EB}"/>
+    <hyperlink ref="A15" r:id="rId8" xr:uid="{373279DF-52F7-4325-963D-2CFF1FC0CD82}"/>
+    <hyperlink ref="A17" r:id="rId9" xr:uid="{57BE27B6-C548-4657-86A6-0EB61F72CB40}"/>
+    <hyperlink ref="A19" r:id="rId10" xr:uid="{D371CDA2-2D04-4DD4-B225-87E802362E06}"/>
+    <hyperlink ref="A21" r:id="rId11" xr:uid="{FB0D88F6-92E3-4433-AEC6-F3F5297114BE}"/>
+    <hyperlink ref="A23" r:id="rId12" xr:uid="{F2D92F8D-E5D3-45D8-9262-2BFC159DC543}"/>
+    <hyperlink ref="A6" r:id="rId13" xr:uid="{B981A00F-221D-462C-B348-4B283B9F4D47}"/>
+    <hyperlink ref="A8" r:id="rId14" xr:uid="{9B175458-30E8-4938-8ABC-F7073D88621D}"/>
+    <hyperlink ref="A10" r:id="rId15" xr:uid="{7324B8EE-E890-4FBA-B1CF-09B764F7B2CC}"/>
+    <hyperlink ref="A12" r:id="rId16" xr:uid="{8D893167-B4BD-434C-8958-C827F23AC77B}"/>
+    <hyperlink ref="A14" r:id="rId17" xr:uid="{9475FAF3-B43C-4BC9-A052-8E4B3EABC24B}"/>
+    <hyperlink ref="A16" r:id="rId18" xr:uid="{5170F69E-34FA-47D6-AEEF-ADFDDE57687B}"/>
+    <hyperlink ref="A18" r:id="rId19" xr:uid="{CB62A601-E999-4D97-8576-41D4FBF024A8}"/>
+    <hyperlink ref="A20" r:id="rId20" xr:uid="{DD7284B4-1210-4865-B889-85C234B26328}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{99B56FB7-25B4-49CA-B674-F186636B10D6}"/>
+    <hyperlink ref="A2" r:id="rId22" xr:uid="{19483A08-CCFB-422F-B6B6-DC8BCFB9EF2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>